<commit_message>
Generar estadísticas de tiempos
</commit_message>
<xml_diff>
--- a/Estadisticas.xlsx
+++ b/Estadisticas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24576" windowHeight="9816"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5196"/>
   </bookViews>
   <sheets>
     <sheet name="17" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="C10:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="I15" sqref="I15:L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,10 +501,10 @@
       </c>
       <c r="J16" s="2">
         <f>L16-K16</f>
-        <v>2479</v>
+        <v>1976</v>
       </c>
       <c r="K16" s="1">
-        <v>430</v>
+        <v>933</v>
       </c>
       <c r="L16" s="3">
         <v>2909</v>
@@ -540,10 +540,10 @@
       </c>
       <c r="D17" s="2">
         <f>F17-E17</f>
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="E17" s="1">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="F17" s="3">
         <v>144</v>
@@ -556,10 +556,10 @@
       </c>
       <c r="J17" s="2">
         <f>L17-K17</f>
-        <v>10907</v>
+        <v>9985</v>
       </c>
       <c r="K17" s="1">
-        <v>729</v>
+        <v>1651</v>
       </c>
       <c r="L17" s="3">
         <f>L16*4</f>
@@ -599,11 +599,11 @@
       </c>
       <c r="D18" s="2">
         <f>(D17/$F$17)*100</f>
-        <v>57.638888888888886</v>
+        <v>43.055555555555557</v>
       </c>
       <c r="E18" s="1">
         <f>(E17/$F$17)*100</f>
-        <v>42.361111111111107</v>
+        <v>56.944444444444443</v>
       </c>
       <c r="F18" s="3">
         <f>($F$17/G17)*100</f>
@@ -614,11 +614,11 @@
       </c>
       <c r="J18" s="2">
         <f>(J16/$L$16)*100</f>
-        <v>85.218288071502229</v>
+        <v>67.927122722585082</v>
       </c>
       <c r="K18" s="1">
         <f>(K16/$L$16)*100</f>
-        <v>14.781711928497765</v>
+        <v>32.072877277414918</v>
       </c>
       <c r="S18" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Actualizacion para añadir errores
</commit_message>
<xml_diff>
--- a/Estadisticas.xlsx
+++ b/Estadisticas.xlsx
@@ -435,7 +435,7 @@
   <dimension ref="C10:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15:L22"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,13 +501,13 @@
       </c>
       <c r="J16" s="2">
         <f>L16-K16</f>
-        <v>1976</v>
+        <v>2893</v>
       </c>
       <c r="K16" s="1">
-        <v>933</v>
+        <v>260</v>
       </c>
       <c r="L16" s="3">
-        <v>2909</v>
+        <v>3153</v>
       </c>
       <c r="T16" s="2" t="s">
         <v>9</v>
@@ -540,10 +540,10 @@
       </c>
       <c r="D17" s="2">
         <f>F17-E17</f>
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="E17" s="1">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="F17" s="3">
         <v>144</v>
@@ -556,14 +556,14 @@
       </c>
       <c r="J17" s="2">
         <f>L17-K17</f>
-        <v>9985</v>
+        <v>12218</v>
       </c>
       <c r="K17" s="1">
-        <v>1651</v>
+        <v>394</v>
       </c>
       <c r="L17" s="3">
         <f>L16*4</f>
-        <v>11636</v>
+        <v>12612</v>
       </c>
       <c r="S17" s="2" t="s">
         <v>4</v>
@@ -599,11 +599,11 @@
       </c>
       <c r="D18" s="2">
         <f>(D17/$F$17)*100</f>
-        <v>43.055555555555557</v>
+        <v>65.972222222222214</v>
       </c>
       <c r="E18" s="1">
         <f>(E17/$F$17)*100</f>
-        <v>56.944444444444443</v>
+        <v>34.027777777777779</v>
       </c>
       <c r="F18" s="3">
         <f>($F$17/G17)*100</f>
@@ -614,11 +614,11 @@
       </c>
       <c r="J18" s="2">
         <f>(J16/$L$16)*100</f>
-        <v>67.927122722585082</v>
+        <v>91.753885188709162</v>
       </c>
       <c r="K18" s="1">
         <f>(K16/$L$16)*100</f>
-        <v>32.072877277414918</v>
+        <v>8.246114811290834</v>
       </c>
       <c r="S18" s="2" t="s">
         <v>2</v>
@@ -640,11 +640,11 @@
       </c>
       <c r="Z18" s="2">
         <f>(Z16/$L$16)*100</f>
-        <v>8.2846338948092129</v>
+        <v>7.6435141135426585</v>
       </c>
       <c r="AA18" s="1">
         <f>(AA16/$L$16)*100</f>
-        <v>11.962873839807495</v>
+        <v>11.037107516650808</v>
       </c>
     </row>
     <row r="20" spans="3:28" x14ac:dyDescent="0.3">

</xml_diff>